<commit_message>
Corrección en el orden de las columnas
Ademas se agrega la columna de tipo, la cual resultó ser distinta a la de concepto
</commit_message>
<xml_diff>
--- a/20240820/20240820_results.xlsx
+++ b/20240820/20240820_results.xlsx
@@ -436,12 +436,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>nombre_cliente</t>
+          <t>fondo</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>operacion_concepto</t>
+          <t>monto</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -451,37 +451,37 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>tipo</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>concepto</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>fecha_operacion</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>fecha_liquidacion</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>monto_operacion</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>cantidad</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>precio</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>nemotecnico</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>cantidad</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>precio</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>forma_pago</t>
         </is>
       </c>
     </row>
@@ -493,47 +493,47 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>12.300.000</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CLP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>VENTA</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>RESCATE</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CLP</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>19/08/2024</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>20/08/2024</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>12.300.000</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>11.247,5571</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>1.093,5708</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>CFMPRULCLP</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>11.247,5571</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>1.093,5708</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>TRANSFERENCIA ELECTRONICA</t>
         </is>
       </c>
     </row>
@@ -545,47 +545,47 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>5.323.478</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CLP</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>VENTA</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>RESCATE</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CLP</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>19/08/2024</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>20/08/2024</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>5.323.478</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>4.867,9773</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>1.093,5708</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>CFMPRULCLP</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>4.867,9773</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>1.093,5708</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>TRANSFERENCIA ELECTRONICA</t>
         </is>
       </c>
     </row>
@@ -597,47 +597,47 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>34.151.465</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CLP</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>VENTA</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>RESCATE</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>CLP</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>19/08/2024</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>20/08/2024</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>34.151.465</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>31.229,3133</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>1.093,5708</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>CFMPRULCLP</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>31.229,3133</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>1.093,5708</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>TRANSFERENCIA ELECTRONICA</t>
         </is>
       </c>
     </row>
@@ -649,47 +649,47 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>15.002.401</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CLP</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>VENTA</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>RESCATE</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>CLP</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>19/08/2024</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>20/08/2024</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>15.002.401</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>13.718,7284</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>1.093,5708</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t>CFMPRULCLP</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>13.718,7284</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>1.093,5708</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>TRANSFERENCIA ELECTRONICA</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se corrigen los formatos de fecha y numero
</commit_message>
<xml_diff>
--- a/20240820/20240820_results.xlsx
+++ b/20240820/20240820_results.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -491,10 +495,8 @@
           <t>FM PRUDENTIAL RENTA INTERNACIONAL</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>12.300.000</t>
-        </is>
+      <c r="B2" t="n">
+        <v>12300000</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -511,25 +513,17 @@
           <t>RESCATE</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>19/08/2024</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>20/08/2024</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>11.247,5571</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>1.093,5708</t>
-        </is>
+      <c r="F2" s="2" t="n">
+        <v>45523</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>45524</v>
+      </c>
+      <c r="H2" t="n">
+        <v>11247.5571</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1093.5708</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -543,10 +537,8 @@
           <t>FM PRUDENTIAL RENTA INTERNACIONAL</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>5.323.478</t>
-        </is>
+      <c r="B3" t="n">
+        <v>5323478</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -563,25 +555,17 @@
           <t>RESCATE</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>19/08/2024</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>20/08/2024</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>4.867,9773</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>1.093,5708</t>
-        </is>
+      <c r="F3" s="2" t="n">
+        <v>45523</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>45524</v>
+      </c>
+      <c r="H3" t="n">
+        <v>4867.9773</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1093.5708</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -595,10 +579,8 @@
           <t>FM PRUDENTIAL RENTA INTERNACIONAL</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>34.151.465</t>
-        </is>
+      <c r="B4" t="n">
+        <v>34151465</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -615,25 +597,17 @@
           <t>RESCATE</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>19/08/2024</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>20/08/2024</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>31.229,3133</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>1.093,5708</t>
-        </is>
+      <c r="F4" s="2" t="n">
+        <v>45523</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>45524</v>
+      </c>
+      <c r="H4" t="n">
+        <v>31229.3133</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1093.5708</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -647,10 +621,8 @@
           <t>FM PRUDENTIAL ACCIONES MUNDO</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>15.002.401</t>
-        </is>
+      <c r="B5" t="n">
+        <v>15002401</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -667,25 +639,17 @@
           <t>RESCATE</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>19/08/2024</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>20/08/2024</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>13.718,7284</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>1.093,5708</t>
-        </is>
+      <c r="F5" s="2" t="n">
+        <v>45523</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>45524</v>
+      </c>
+      <c r="H5" t="n">
+        <v>13718.7284</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1093.5708</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>

</xml_diff>